<commit_message>
complete bbs's dianzan,attention, collection
</commit_message>
<xml_diff>
--- a/数据库设计/需求分析/数据字典.xlsx
+++ b/数据库设计/需求分析/数据字典.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="用户" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="206">
   <si>
     <t xml:space="preserve">用户数据字典</t>
   </si>
@@ -223,7 +223,25 @@
     <t xml:space="preserve">Zjhfr_id</t>
   </si>
   <si>
-    <t xml:space="preserve">引用用户表的Id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">引用用户表的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">置顶</t>
@@ -235,7 +253,44 @@
     <t xml:space="preserve">Boolean</t>
   </si>
   <si>
-    <t xml:space="preserve">true表示置顶，false表示不置顶</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">表示置顶，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">表示不置顶</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">点赞数</t>
@@ -253,7 +308,25 @@
     <t xml:space="preserve">Board_type</t>
   </si>
   <si>
-    <t xml:space="preserve">主题所属的版块；引用版块表的Type</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">主题所属的版块；引用版块表的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Type</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">发表人编号</t>
@@ -280,6 +353,33 @@
     <t xml:space="preserve">多少用户收藏这个主题</t>
   </si>
   <si>
+    <t xml:space="preserve">学院类型</t>
+  </si>
+  <si>
+    <t xml:space="preserve">College_type</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">引用学院表的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Id</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">回复数据字典</t>
   </si>
   <si>
@@ -310,7 +410,82 @@
     <t xml:space="preserve">版块数据字典</t>
   </si>
   <si>
-    <t xml:space="preserve">0：活动区；-1：问题区；-2：话题区；结合用户表的Rank区分每个版块的管理员</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：活动区；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：问题区；</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：话题区；结合用户表的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Rank</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">区分每个版块的管理员</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">公告</t>
@@ -349,7 +524,25 @@
     <t xml:space="preserve">Yh_id</t>
   </si>
   <si>
-    <t xml:space="preserve">引用主题表Theme_id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">引用主题表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Theme_id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">关注数据字典</t>
@@ -367,16 +560,70 @@
     <t xml:space="preserve">Ox_id</t>
   </si>
   <si>
-    <t xml:space="preserve">发布课程数据字典（Submit_Les)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">课程id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">发布课程数据字典（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Submit_Les)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">课程</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Les_Id  (Primary Key)</t>
   </si>
   <si>
-    <t xml:space="preserve">用户id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">用户</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Person_Id</t>
@@ -385,7 +632,25 @@
     <t xml:space="preserve">Foreign Key</t>
   </si>
   <si>
-    <t xml:space="preserve">课程标签id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">课程标签</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Label_Id</t>
@@ -397,7 +662,25 @@
     <t xml:space="preserve">Label_Kind</t>
   </si>
   <si>
-    <t xml:space="preserve">(1,2,3)分别代表理论，项目，技能</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(1,2,3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">分别代表理论，项目，技能</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">具体名称</t>
@@ -475,7 +758,63 @@
     <t xml:space="preserve">Les_Status</t>
   </si>
   <si>
-    <t xml:space="preserve">1代表正在进行，2代表招收中，3代表已结课</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">代表正在进行，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">代表招收中，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">代表已结课</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ChoiceLes_Field</t>
@@ -484,7 +823,25 @@
     <t xml:space="preserve">Les_Id</t>
   </si>
   <si>
-    <t xml:space="preserve">用户Id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">用户</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">订课者</t>
@@ -517,10 +874,46 @@
     <t xml:space="preserve">星级数</t>
   </si>
   <si>
-    <t xml:space="preserve">评论数据字典(Comment_Field)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">评论id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">评论数据字典</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(Comment_Field)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">评论</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Comment_Id</t>
@@ -550,7 +943,25 @@
     <t xml:space="preserve">Comment </t>
   </si>
   <si>
-    <t xml:space="preserve">回复数据字典(Answer_Field)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">回复数据字典</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(Answer_Field)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Comment_id </t>
@@ -562,7 +973,25 @@
     <t xml:space="preserve">Answer</t>
   </si>
   <si>
-    <t xml:space="preserve">标签数据字典(Label_Field)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">标签数据字典</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(Label_Field)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">课程标签</t>
@@ -574,7 +1003,54 @@
     <t xml:space="preserve">类别</t>
   </si>
   <si>
-    <t xml:space="preserve">1，2，3</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">名字</t>
@@ -583,10 +1059,46 @@
     <t xml:space="preserve">Label_Name</t>
   </si>
   <si>
-    <t xml:space="preserve">学院数据字典(College_Field)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">学院id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">学院数据字典</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(College_Field)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">学院</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">College_Id</t>
@@ -607,7 +1119,25 @@
     <t xml:space="preserve">Community_field</t>
   </si>
   <si>
-    <t xml:space="preserve">社团id</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">社团</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="等线"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">id</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Com_Id</t>
@@ -650,7 +1180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -672,6 +1202,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -727,7 +1263,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -736,12 +1272,20 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -752,15 +1296,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -768,12 +1312,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -788,7 +1336,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="常规 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -800,18 +1348,18 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,10 +1375,10 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="3" t="n">
@@ -841,7 +1389,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -853,12 +1401,12 @@
       <c r="D3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -870,12 +1418,12 @@
       <c r="D4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -887,12 +1435,12 @@
       <c r="D5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
@@ -901,9 +1449,10 @@
       <c r="C6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -917,7 +1466,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -931,7 +1480,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -940,9 +1489,10 @@
       <c r="C9" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="D9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
@@ -956,7 +1506,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
@@ -970,7 +1520,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -982,12 +1532,12 @@
       <c r="D12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="0" t="s">
@@ -1001,7 +1551,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="0" t="s">
@@ -1013,12 +1563,12 @@
       <c r="D14" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="0" t="s">
@@ -1030,7 +1580,7 @@
       <c r="D15" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1061,12 +1611,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1092,17 +1642,17 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>116</v>
+        <v>176</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="E4" s="12"/>
+        <v>177</v>
+      </c>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
@@ -1111,7 +1661,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1142,12 +1692,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1172,33 +1722,33 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>177</v>
+      <c r="A3" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>179</v>
+      <c r="A4" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>181</v>
+      <c r="A5" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1223,17 +1773,17 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1258,25 +1808,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>184</v>
+      <c r="A3" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>186</v>
+      <c r="A4" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>3</v>
@@ -1286,11 +1836,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>188</v>
+      <c r="A5" s="5" t="s">
+        <v>191</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>16</v>
@@ -1323,17 +1873,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -1353,70 +1903,70 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>191</v>
+      <c r="A3" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>193</v>
+      <c r="A4" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>195</v>
+      <c r="A5" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>197</v>
+      <c r="A6" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>200</v>
+      <c r="A7" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>202</v>
+      <c r="E7" s="5" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1438,30 +1988,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:16"/>
+  <dimension ref="1:17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="12.0604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="4" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="6" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -2483,19 +3033,19 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="0"/>
@@ -3519,19 +4069,19 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="10" t="s">
         <v>49</v>
       </c>
       <c r="F3" s="0"/>
@@ -4555,16 +5105,16 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="12" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="0"/>
@@ -5589,16 +6139,16 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="0"/>
@@ -6623,16 +7173,16 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="7" t="n">
         <v>10</v>
       </c>
       <c r="E6" s="0"/>
@@ -7656,169 +8206,186 @@
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
-    <row r="7" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+    <row r="7" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10" t="n">
+      <c r="D7" s="7" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="10" t="n">
+      <c r="D8" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="10" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="7" t="n">
         <v>8</v>
       </c>
       <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="10" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -7848,22 +8415,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="11.693023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="10.2139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="32.3674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="4" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="6" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="0"/>
       <c r="G1" s="0"/>
       <c r="H1" s="0"/>
@@ -8885,19 +9452,19 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F2" s="0"/>
@@ -9921,19 +10488,19 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="10" t="s">
         <v>63</v>
       </c>
       <c r="F3" s="0"/>
@@ -10956,99 +11523,99 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="9" t="s">
+    <row r="4" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="10" t="n">
+      <c r="D4" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>87</v>
+      <c r="E4" s="10" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="7" t="n">
         <v>10</v>
       </c>
       <c r="E5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>88</v>
+      <c r="E6" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="7" t="n">
         <v>8</v>
       </c>
       <c r="E8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="10" t="s">
         <v>80</v>
       </c>
     </row>
@@ -11079,117 +11646,117 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="4" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="42.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="6" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>92</v>
+      <c r="E3" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="7" t="n">
         <v>8</v>
       </c>
       <c r="E5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="7" t="n">
         <v>8</v>
       </c>
       <c r="E6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>101</v>
+      <c r="E7" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -11219,70 +11786,70 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="4" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="4" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="6" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="6" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>105</v>
+      <c r="E4" s="10" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -11312,69 +11879,69 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="4" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="17.8418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="4" width="9.22790697674419"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="6" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="6" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
         <v>63</v>
       </c>
     </row>
@@ -11405,12 +11972,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -11435,109 +12002,109 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>112</v>
+      <c r="A3" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>114</v>
+      <c r="A4" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>116</v>
+      <c r="E4" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>118</v>
+      <c r="A5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>116</v>
+      <c r="E5" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>120</v>
+      <c r="A6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>123</v>
+      <c r="A7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>125</v>
+      <c r="A8" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>128</v>
+      <c r="A9" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>130</v>
+      <c r="A10" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>3</v>
@@ -11547,77 +12114,77 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>132</v>
+      <c r="A11" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>134</v>
+      <c r="A12" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>136</v>
+      <c r="A13" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>138</v>
+      <c r="A14" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>140</v>
+      <c r="A15" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>142</v>
+      <c r="A16" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>145</v>
+      <c r="A17" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -11647,17 +12214,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -11677,67 +12244,67 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>112</v>
+      <c r="A3" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>150</v>
+      <c r="A4" s="5" t="s">
+        <v>153</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>151</v>
+      <c r="E4" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>152</v>
+      <c r="A5" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>154</v>
+      <c r="A6" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>158</v>
+      <c r="A7" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>160</v>
+      <c r="E7" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -11767,12 +12334,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -11797,67 +12364,67 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>162</v>
+      <c r="A3" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>112</v>
+      <c r="A4" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>114</v>
+      <c r="A5" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>169</v>
+        <v>119</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>170</v>
+      <c r="A7" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>